<commit_message>
Pulling maps out of state. However, maps are not currently rendering
</commit_message>
<xml_diff>
--- a/colormap.xlsx
+++ b/colormap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="897" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="897"/>
   </bookViews>
   <sheets>
     <sheet name="MasterMaps" sheetId="19" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="54">
   <si>
     <t>B</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>streched</t>
+  </si>
+  <si>
+    <t>discrete</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1024,7 +1033,7 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1034,8 +1043,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1045,8 +1057,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1056,8 +1071,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1067,8 +1085,11 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1078,8 +1099,11 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1089,8 +1113,11 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1100,8 +1127,11 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1111,8 +1141,11 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1122,8 +1155,11 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1133,8 +1169,11 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1144,8 +1183,11 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1155,8 +1197,11 @@
       <c r="C12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1166,8 +1211,11 @@
       <c r="C13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1177,8 +1225,11 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1188,8 +1239,11 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1199,8 +1253,11 @@
       <c r="C16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1210,8 +1267,11 @@
       <c r="C17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1221,8 +1281,11 @@
       <c r="C18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1232,8 +1295,11 @@
       <c r="C19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1243,8 +1309,11 @@
       <c r="C20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1254,8 +1323,11 @@
       <c r="C21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1264,6 +1336,9 @@
       </c>
       <c r="C22" t="s">
         <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +2280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>